<commit_message>
added transferibility data and nb that tranin ML
</commit_message>
<xml_diff>
--- a/data/transferability.xlsx
+++ b/data/transferability.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nairrg\WORKS\ML\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barradd/Documents/GitHub/machine_learning_chem_RGS/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF408A5-2C63-4BB0-9238-69FEE916CB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13153610-5F10-224E-A5AD-781054CC27CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="30915" windowHeight="16876" activeTab="1" xr2:uid="{A53A9583-D0F7-47BF-8E80-ECEBF6ED7B52}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30920" windowHeight="16880" activeTab="1" xr2:uid="{A53A9583-D0F7-47BF-8E80-ECEBF6ED7B52}"/>
   </bookViews>
   <sheets>
     <sheet name="transferability" sheetId="1" r:id="rId1"/>
-    <sheet name="additivity" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="additivity" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="132">
   <si>
     <t xml:space="preserve">Transferability </t>
   </si>
@@ -1071,7 +1072,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -1185,11 +1186,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1198,32 +1198,32 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1374,9 +1374,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1414,7 +1414,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1520,7 +1520,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1662,7 +1662,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1672,562 +1672,562 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0404153-F32B-497B-92C4-229AA4341A27}">
   <dimension ref="B3:L43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="5" width="11.5" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="14" t="s">
+    <row r="3" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E14" s="2" t="s">
+    <row r="14" spans="2:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="E14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="3" t="s">
+      <c r="F14" s="1"/>
+      <c r="G14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="3" t="s">
+      <c r="H14" s="1"/>
+      <c r="I14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2" t="s">
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
+    <row r="16" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+    <row r="19" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>28.3</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>20.5</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>26.7</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <v>40.4</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="6">
         <v>42.6</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
+    <row r="20" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>23</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="6">
         <v>16.7</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>22.5</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <v>32.200000000000003</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="6">
         <v>33.5</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+    <row r="21" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>21.2</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>14.5</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>19.899999999999999</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <v>31.8</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="6">
         <v>35.200000000000003</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
+    <row r="22" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>18</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="6">
         <v>13</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="6">
         <v>16.899999999999999</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="6">
         <v>25</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="6">
         <v>29.2</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+    <row r="23" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>15.2</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="6">
         <v>10.9</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="6">
         <v>13</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="6">
         <v>19.399999999999999</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="6">
         <v>12.5</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
+    <row r="24" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B24" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5">
         <v>13.8</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="6">
         <v>9.6</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
         <v>11.8</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="6">
         <v>17.600000000000001</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="6">
         <v>17.5</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
+    <row r="25" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B25" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>11</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="6">
         <v>8.3000000000000007</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="6">
         <v>7.8</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="6">
         <v>13.4</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="6">
         <v>13.4</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
+    <row r="26" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="5">
         <v>9.6999999999999993</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="6">
         <v>6.4</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="6">
         <v>7.9</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="6">
         <v>13.1</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="6">
         <v>11.6</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
+    <row r="27" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B27" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="5">
         <v>8.3000000000000007</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <v>8.5</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="6">
         <v>7.5</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="6">
         <v>11.3</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
+    <row r="28" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="5">
         <v>7</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="6">
         <v>5.3</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="6">
         <v>6.5</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="6">
         <v>8.6999999999999993</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="6">
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
+    <row r="29" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="5">
         <v>5.9</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="6">
         <v>4.9000000000000004</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="6">
         <v>7.1</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="6">
         <v>8</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="6">
         <v>9.4</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
+    <row r="30" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B30" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="5">
         <v>3.5</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="6">
         <v>2.1</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="6">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="6">
         <v>5.9</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G30" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
+    <row r="31" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B31" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="5">
         <v>1.8</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="6">
         <v>1.2</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="6">
         <v>1.4</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="6">
         <v>1.8</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="6">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
+    <row r="32" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B32" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="5">
         <v>1</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="6">
         <v>0.4</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E32" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="6">
         <v>0</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="G32" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
+    <row r="33" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B33" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="5">
         <v>0.2</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F33" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G33" s="7" t="s">
+      <c r="G33" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
+    <row r="34" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B34" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="5">
         <v>0</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="6">
         <v>0</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="6">
         <v>0</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="6">
         <v>0</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G34" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
+    <row r="35" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B35" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G35" s="7" t="s">
+      <c r="G35" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
+    <row r="36" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B36" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F36" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G36" s="7" t="s">
+      <c r="G36" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
+    <row r="37" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B37" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G37" s="7" t="s">
+      <c r="G37" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B38" s="5" t="s">
+    <row r="38" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B38" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E38" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F38" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G38" s="7" t="s">
+      <c r="G38" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="5" t="s">
+    <row r="39" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B39" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E39" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="F39" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G39" s="7" t="s">
+      <c r="G39" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="5" t="s">
+    <row r="40" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B40" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D40" s="6">
         <v>2.4</v>
       </c>
-      <c r="E40" s="7" t="s">
+      <c r="E40" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F40" s="7">
+      <c r="F40" s="6">
         <v>0.4</v>
       </c>
-      <c r="G40" s="7" t="s">
+      <c r="G40" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="5" t="s">
+    <row r="41" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B41" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="E41" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="F41" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G41" s="7" t="s">
+      <c r="G41" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B42" s="5" t="s">
+    <row r="42" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B42" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="F42" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G42" s="7" t="s">
+      <c r="G42" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="5" t="s">
+    <row r="43" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B43" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="E43" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F43" s="7" t="s">
+      <c r="F43" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G43" s="7" t="s">
+      <c r="G43" s="6" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2238,65 +2238,600 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E743AA1A-C9B2-3F4B-BC46-3F53546BC2F0}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5">
+        <v>28.3</v>
+      </c>
+      <c r="C2" s="6">
+        <v>20.5</v>
+      </c>
+      <c r="D2" s="6">
+        <v>26.7</v>
+      </c>
+      <c r="E2" s="6">
+        <v>40.4</v>
+      </c>
+      <c r="F2" s="6">
+        <v>42.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5">
+        <v>23</v>
+      </c>
+      <c r="C3" s="6">
+        <v>16.7</v>
+      </c>
+      <c r="D3" s="6">
+        <v>22.5</v>
+      </c>
+      <c r="E3" s="6">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="F3" s="6">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5">
+        <v>21.2</v>
+      </c>
+      <c r="C4" s="6">
+        <v>14.5</v>
+      </c>
+      <c r="D4" s="6">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="E4" s="6">
+        <v>31.8</v>
+      </c>
+      <c r="F4" s="6">
+        <v>35.200000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5">
+        <v>18</v>
+      </c>
+      <c r="C5" s="6">
+        <v>13</v>
+      </c>
+      <c r="D5" s="6">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="E5" s="6">
+        <v>25</v>
+      </c>
+      <c r="F5" s="6">
+        <v>29.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5">
+        <v>15.2</v>
+      </c>
+      <c r="C6" s="6">
+        <v>10.9</v>
+      </c>
+      <c r="D6" s="6">
+        <v>13</v>
+      </c>
+      <c r="E6" s="6">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="F6" s="6">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5">
+        <v>13.8</v>
+      </c>
+      <c r="C7" s="6">
+        <v>9.6</v>
+      </c>
+      <c r="D7" s="6">
+        <v>11.8</v>
+      </c>
+      <c r="E7" s="6">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="F7" s="6">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D8" s="6">
+        <v>7.8</v>
+      </c>
+      <c r="E8" s="6">
+        <v>13.4</v>
+      </c>
+      <c r="F8" s="6">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="5">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="C9" s="6">
+        <v>6.4</v>
+      </c>
+      <c r="D9" s="6">
+        <v>7.9</v>
+      </c>
+      <c r="E9" s="6">
+        <v>13.1</v>
+      </c>
+      <c r="F9" s="6">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="5">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C10" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="D10" s="6">
+        <v>7.5</v>
+      </c>
+      <c r="E10" s="6">
+        <v>11.3</v>
+      </c>
+      <c r="F10" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5">
+        <v>7</v>
+      </c>
+      <c r="C11" s="6">
+        <v>5.3</v>
+      </c>
+      <c r="D11" s="6">
+        <v>6.5</v>
+      </c>
+      <c r="E11" s="6">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F11" s="6">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="5">
+        <v>5.9</v>
+      </c>
+      <c r="C12" s="6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D12" s="6">
+        <v>7.1</v>
+      </c>
+      <c r="E12" s="6">
+        <v>8</v>
+      </c>
+      <c r="F12" s="6">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="D13" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E13" s="6">
+        <v>5.9</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1.4</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="F14" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F36DF037-54E7-4BE6-8D37-6767B05780BB}">
   <dimension ref="B2:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="12" width="12.140625" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="12" width="12.1640625" customWidth="1"/>
+    <col min="13" max="13" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="14" t="s">
+    <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F16" s="1" t="s">
         <v>75</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="L16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="N16" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="F17" s="15" t="s">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="F17" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15" t="s">
+      <c r="G17" s="12"/>
+      <c r="H17" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="J17" s="15" t="s">
+      <c r="J17" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="L17" s="15" t="s">
+      <c r="L17" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="N17" s="15" t="s">
+      <c r="N17" s="12" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
+    <row r="19" spans="2:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B19" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="13" t="s">
@@ -2307,551 +2842,551 @@
         <v>4</v>
       </c>
       <c r="F19" s="13"/>
-      <c r="I19" s="10" t="s">
+      <c r="I19" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="J19" s="11" t="s">
+      <c r="J19" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11" t="s">
+      <c r="K19" s="14"/>
+      <c r="L19" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11" t="s">
+      <c r="M19" s="14"/>
+      <c r="N19" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="O19" s="11"/>
-    </row>
-    <row r="20" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="12" t="s">
+      <c r="O19" s="14"/>
+    </row>
+    <row r="20" spans="2:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B20" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="K20" s="10" t="s">
+      <c r="K20" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="L20" s="10" t="s">
+      <c r="L20" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="M20" s="10" t="s">
+      <c r="M20" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="N20" s="10" t="s">
+      <c r="N20" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="O20" s="10" t="s">
+      <c r="O20" s="9" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+    <row r="21" spans="2:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>63.6</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>65.7</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>59.7</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <v>63.7</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="J21" s="9">
+      <c r="J21" s="8">
         <v>50.8</v>
       </c>
-      <c r="K21" s="9">
+      <c r="K21" s="8">
         <v>51.7</v>
       </c>
-      <c r="L21" s="9">
+      <c r="L21" s="8">
         <v>58.6</v>
       </c>
-      <c r="M21" s="9">
+      <c r="M21" s="8">
         <v>62.4</v>
       </c>
-      <c r="N21" s="9">
+      <c r="N21" s="8">
         <v>61.7</v>
       </c>
-      <c r="O21" s="9">
+      <c r="O21" s="8">
         <v>65.2</v>
       </c>
     </row>
-    <row r="22" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
+    <row r="22" spans="2:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>54</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="6">
         <v>59.5</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="6">
         <v>50.6</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="6">
         <v>57.5</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I22" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="J22" s="9">
+      <c r="J22" s="8">
         <v>41.4</v>
       </c>
-      <c r="K22" s="9">
+      <c r="K22" s="8">
         <v>41.8</v>
       </c>
-      <c r="L22" s="9">
+      <c r="L22" s="8">
         <v>44.2</v>
       </c>
-      <c r="M22" s="9">
+      <c r="M22" s="8">
         <v>46.1</v>
       </c>
-      <c r="N22" s="9">
+      <c r="N22" s="8">
         <v>47.9</v>
       </c>
-      <c r="O22" s="9">
+      <c r="O22" s="8">
         <v>49.7</v>
       </c>
     </row>
-    <row r="23" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+    <row r="23" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="6">
         <v>41.4</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="6">
         <v>39.6</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="6">
         <v>35.5</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="6">
         <v>35.799999999999997</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="I23" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="J23" s="9">
+      <c r="J23" s="8">
         <v>16.2</v>
       </c>
-      <c r="K23" s="9">
+      <c r="K23" s="8">
         <v>16.7</v>
       </c>
-      <c r="L23" s="9">
+      <c r="L23" s="8">
         <v>20.2</v>
       </c>
-      <c r="M23" s="9">
+      <c r="M23" s="8">
         <v>18</v>
       </c>
-      <c r="N23" s="9">
+      <c r="N23" s="8">
         <v>18.100000000000001</v>
       </c>
-      <c r="O23" s="9">
+      <c r="O23" s="8">
         <v>19.5</v>
       </c>
     </row>
-    <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
+    <row r="24" spans="2:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B24" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6">
         <v>21</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="6">
         <v>26.7</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
         <v>19.600000000000001</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="6">
         <v>25.1</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="I24" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="8">
         <v>44</v>
       </c>
-      <c r="K24" s="9">
+      <c r="K24" s="8">
         <v>44.1</v>
       </c>
-      <c r="L24" s="9">
+      <c r="L24" s="8">
         <v>40.200000000000003</v>
       </c>
-      <c r="M24" s="9">
+      <c r="M24" s="8">
         <v>40.700000000000003</v>
       </c>
-      <c r="N24" s="9">
+      <c r="N24" s="8">
         <v>27.6</v>
       </c>
-      <c r="O24" s="9">
+      <c r="O24" s="8">
         <v>27.5</v>
       </c>
     </row>
-    <row r="25" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
+    <row r="25" spans="2:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B25" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="I25" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="J25" s="9">
+      <c r="J25" s="8">
         <v>40.6</v>
       </c>
-      <c r="K25" s="9">
+      <c r="K25" s="8">
         <v>40.6</v>
       </c>
-      <c r="L25" s="9">
+      <c r="L25" s="8">
         <v>25.6</v>
       </c>
-      <c r="M25" s="9">
+      <c r="M25" s="8">
         <v>25.6</v>
       </c>
-      <c r="N25" s="9">
+      <c r="N25" s="8">
         <v>20.7</v>
       </c>
-      <c r="O25" s="9">
+      <c r="O25" s="8">
         <v>20.3</v>
       </c>
     </row>
-    <row r="26" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
+    <row r="26" spans="2:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B26" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="I26" s="8" t="s">
+      <c r="I26" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="J26" s="9">
+      <c r="J26" s="8">
         <v>3.9</v>
       </c>
-      <c r="K26" s="9">
+      <c r="K26" s="8">
         <v>3.9</v>
       </c>
-      <c r="L26" s="9" t="s">
+      <c r="L26" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="M26" s="9" t="s">
+      <c r="M26" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="N26" s="9" t="s">
+      <c r="N26" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="O26" s="9" t="s">
+      <c r="O26" s="8" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
+    <row r="27" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="I27" s="8" t="s">
+      <c r="I27" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="J27" s="9">
+      <c r="J27" s="8">
         <v>37</v>
       </c>
-      <c r="K27" s="9">
+      <c r="K27" s="8">
         <v>37</v>
       </c>
-      <c r="L27" s="9">
+      <c r="L27" s="8">
         <v>28.6</v>
       </c>
-      <c r="M27" s="9">
+      <c r="M27" s="8">
         <v>27.6</v>
       </c>
-      <c r="N27" s="9">
+      <c r="N27" s="8">
         <v>13.5</v>
       </c>
-      <c r="O27" s="9">
+      <c r="O27" s="8">
         <v>11.9</v>
       </c>
     </row>
-    <row r="28" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
+    <row r="28" spans="2:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="I28" s="8" t="s">
+      <c r="I28" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="J28" s="9">
+      <c r="J28" s="8">
         <v>23</v>
       </c>
-      <c r="K28" s="9">
+      <c r="K28" s="8">
         <v>22.9</v>
       </c>
-      <c r="L28" s="9">
+      <c r="L28" s="8">
         <v>9.1999999999999993</v>
       </c>
-      <c r="M28" s="9">
+      <c r="M28" s="8">
         <v>7.8</v>
       </c>
-      <c r="N28" s="9" t="s">
+      <c r="N28" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="O28" s="9" t="s">
+      <c r="O28" s="8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
+    <row r="29" spans="2:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B29" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="6">
         <v>53</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="6">
         <v>51.3</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="6">
         <v>48.6</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="6">
         <v>53.9</v>
       </c>
-      <c r="I29" s="8" t="s">
+      <c r="I29" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="J29" s="9">
+      <c r="J29" s="8">
         <v>49.5</v>
       </c>
-      <c r="K29" s="9">
+      <c r="K29" s="8">
         <v>50.2</v>
       </c>
-      <c r="L29" s="9">
+      <c r="L29" s="8">
         <v>54.3</v>
       </c>
-      <c r="M29" s="9">
+      <c r="M29" s="8">
         <v>63.5</v>
       </c>
-      <c r="N29" s="9">
+      <c r="N29" s="8">
         <v>58.6</v>
       </c>
-      <c r="O29" s="9">
+      <c r="O29" s="8">
         <v>62.6</v>
       </c>
     </row>
-    <row r="30" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
+    <row r="30" spans="2:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B30" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="6">
         <v>30</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="6">
         <v>28.3</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="6">
         <v>25.6</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="6">
         <v>28.4</v>
       </c>
-      <c r="I30" s="8" t="s">
+      <c r="I30" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="J30" s="9">
+      <c r="J30" s="8">
         <v>45.2</v>
       </c>
-      <c r="K30" s="9">
+      <c r="K30" s="8">
         <v>45.1</v>
       </c>
-      <c r="L30" s="9">
+      <c r="L30" s="8">
         <v>26.8</v>
       </c>
-      <c r="M30" s="9">
+      <c r="M30" s="8">
         <v>33.4</v>
       </c>
-      <c r="N30" s="9">
+      <c r="N30" s="8">
         <v>18.100000000000001</v>
       </c>
-      <c r="O30" s="9">
+      <c r="O30" s="8">
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="31" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
+    <row r="31" spans="2:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B31" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="6">
         <v>4</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="6">
         <v>8.4</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="6">
         <v>7</v>
       </c>
-      <c r="I31" s="8" t="s">
+      <c r="I31" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="J31" s="9">
+      <c r="J31" s="8">
         <v>25.3</v>
       </c>
-      <c r="K31" s="9">
+      <c r="K31" s="8">
         <v>25.2</v>
       </c>
-      <c r="L31" s="9">
+      <c r="L31" s="8">
         <v>13.9</v>
       </c>
-      <c r="M31" s="9">
+      <c r="M31" s="8">
         <v>21.2</v>
       </c>
-      <c r="N31" s="9" t="s">
+      <c r="N31" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="O31" s="9" t="s">
+      <c r="O31" s="8" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
+    <row r="32" spans="2:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B32" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="6">
         <v>23</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="6">
         <v>28.6</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="6">
         <v>20</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="6">
         <v>28.3</v>
       </c>
-      <c r="I32" s="8" t="s">
+      <c r="I32" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="J32" s="9">
+      <c r="J32" s="8">
         <v>14.4</v>
       </c>
-      <c r="K32" s="9">
+      <c r="K32" s="8">
         <v>14.5</v>
       </c>
-      <c r="L32" s="9">
+      <c r="L32" s="8">
         <v>14.8</v>
       </c>
-      <c r="M32" s="9">
+      <c r="M32" s="8">
         <v>21.2</v>
       </c>
-      <c r="N32" s="9">
+      <c r="N32" s="8">
         <v>16.5</v>
       </c>
-      <c r="O32" s="9">
+      <c r="O32" s="8">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
+    <row r="33" spans="2:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="B33" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F33" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="I33" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="J33" s="9">
+      <c r="J33" s="8">
         <v>45.8</v>
       </c>
-      <c r="K33" s="9">
+      <c r="K33" s="8">
         <v>45.6</v>
       </c>
-      <c r="L33" s="9">
+      <c r="L33" s="8">
         <v>51</v>
       </c>
-      <c r="M33" s="9">
+      <c r="M33" s="8">
         <v>52.1</v>
       </c>
-      <c r="N33" s="9" t="s">
+      <c r="N33" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="O33" s="9" t="s">
+      <c r="O33" s="8" t="s">
         <v>127</v>
       </c>
     </row>

</xml_diff>